<commit_message>
Airbrush blocks in AMAU
</commit_message>
<xml_diff>
--- a/Tallaght Tallght Model_Original/control.xlsx
+++ b/Tallaght Tallght Model_Original/control.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sim Runs (2)" sheetId="33" r:id="rId1"/>
-    <sheet name="Zone1" sheetId="1" state="hidden" r:id="rId2"/>
+    <sheet name="Zone1" sheetId="1" r:id="rId2"/>
     <sheet name="Resus" sheetId="21" r:id="rId3"/>
     <sheet name="ZONE (1) MAJOR" sheetId="23" r:id="rId4"/>
     <sheet name="Zone2" sheetId="2" state="hidden" r:id="rId5"/>
@@ -1274,12 +1274,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1295,7 +1289,13 @@
     <xf numFmtId="0" fontId="23" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1650,61 +1650,29 @@
       <c r="A1" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="37">
-        <v>4.4710683340905222</v>
-      </c>
-      <c r="C1" s="37">
-        <v>9.8183659296948456</v>
-      </c>
-      <c r="D1" s="37">
-        <v>2.9432690210607175</v>
-      </c>
-      <c r="E1" s="37">
-        <v>5.5270913428264761</v>
-      </c>
-      <c r="F1" s="37">
-        <v>9.8440354344834908</v>
-      </c>
-      <c r="G1" s="37">
-        <v>3.8151997202728345</v>
-      </c>
-      <c r="H1" s="37">
-        <v>3.5037154970923434</v>
-      </c>
-      <c r="I1" s="37">
-        <v>3.0882827704190272</v>
-      </c>
-      <c r="J1" s="37">
-        <v>3.971077314599825</v>
-      </c>
-      <c r="K1" s="38">
-        <v>19</v>
-      </c>
-      <c r="L1" s="38">
-        <v>115</v>
-      </c>
-      <c r="M1" s="38">
-        <v>9</v>
-      </c>
-      <c r="N1" s="39">
-        <v>4.6039190531083305</v>
-      </c>
-      <c r="O1" s="39">
-        <v>0.97073973496402666</v>
-      </c>
-      <c r="P1" s="39">
-        <v>0.8558730301571259</v>
-      </c>
-      <c r="Q1" s="39">
-        <v>84.692687591441583</v>
-      </c>
-      <c r="R1" s="40">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="40" t="e">
         <f>K1/L1</f>
-        <v>0.16521739130434782</v>
-      </c>
-      <c r="S1" s="40">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S1" s="40" t="e">
         <f>M1/K1</f>
-        <v>0.47368421052631576</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -1966,69 +1934,69 @@
       <c r="K12" s="43"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B13" s="44">
+      <c r="B13" s="44" t="e">
         <f t="shared" ref="B13:L13" si="2">AVERAGE(B1:B10)</f>
-        <v>4.4710683340905222</v>
-      </c>
-      <c r="C13" s="44">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C13" s="44" t="e">
         <f t="shared" si="2"/>
-        <v>9.8183659296948456</v>
-      </c>
-      <c r="D13" s="44">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D13" s="44" t="e">
         <f t="shared" si="2"/>
-        <v>2.9432690210607175</v>
-      </c>
-      <c r="E13" s="44">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E13" s="44" t="e">
         <f t="shared" si="2"/>
-        <v>5.5270913428264761</v>
-      </c>
-      <c r="F13" s="44">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F13" s="44" t="e">
         <f t="shared" si="2"/>
-        <v>9.8440354344834908</v>
-      </c>
-      <c r="G13" s="44">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G13" s="44" t="e">
         <f t="shared" si="2"/>
-        <v>3.8151997202728345</v>
-      </c>
-      <c r="H13" s="44">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H13" s="44" t="e">
         <f t="shared" si="2"/>
-        <v>3.5037154970923434</v>
-      </c>
-      <c r="I13" s="44">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I13" s="44" t="e">
         <f t="shared" si="2"/>
-        <v>3.0882827704190272</v>
-      </c>
-      <c r="J13" s="44">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J13" s="44" t="e">
         <f t="shared" si="2"/>
-        <v>3.971077314599825</v>
-      </c>
-      <c r="K13" s="44">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K13" s="44" t="e">
         <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
-      <c r="L13" s="44">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L13" s="44" t="e">
         <f t="shared" si="2"/>
-        <v>115</v>
-      </c>
-      <c r="M13" s="44">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M13" s="44" t="e">
         <f t="shared" ref="M13:S13" si="3">AVERAGE(M1:M10)</f>
-        <v>9</v>
-      </c>
-      <c r="N13" s="44">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N13" s="44" t="e">
         <f t="shared" si="3"/>
-        <v>4.6039190531083305</v>
-      </c>
-      <c r="O13" s="44">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O13" s="44" t="e">
         <f t="shared" si="3"/>
-        <v>0.97073973496402666</v>
-      </c>
-      <c r="P13" s="44">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P13" s="44" t="e">
         <f t="shared" si="3"/>
-        <v>0.8558730301571259</v>
-      </c>
-      <c r="Q13" s="44">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q13" s="44" t="e">
         <f t="shared" si="3"/>
-        <v>84.692687591441583</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="R13" s="44" t="e">
         <f t="shared" si="3"/>
@@ -2155,11 +2123,11 @@
       <c r="A1" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="105"/>
-      <c r="D1" s="99"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="105"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="78" t="s">
@@ -9604,7 +9572,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="100" t="s">
+      <c r="A19" s="98" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="63">
@@ -9639,7 +9607,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="101"/>
+      <c r="A20" s="99"/>
       <c r="B20" s="63">
         <v>2</v>
       </c>
@@ -9672,7 +9640,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="101"/>
+      <c r="A21" s="99"/>
       <c r="B21" s="63">
         <v>2</v>
       </c>
@@ -10160,7 +10128,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="102" t="s">
+      <c r="A19" s="100" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="63">
@@ -10200,7 +10168,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="103"/>
+      <c r="A20" s="101"/>
       <c r="B20" s="63">
         <v>7</v>
       </c>
@@ -10238,7 +10206,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="104"/>
+      <c r="A21" s="102"/>
       <c r="B21" s="63">
         <v>5</v>
       </c>
@@ -11236,7 +11204,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="102" t="s">
+      <c r="A19" s="100" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="63">
@@ -11274,7 +11242,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="103"/>
+      <c r="A20" s="101"/>
       <c r="B20" s="63">
         <v>7</v>
       </c>
@@ -11310,7 +11278,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="104"/>
+      <c r="A21" s="102"/>
       <c r="B21" s="63">
         <v>5</v>
       </c>
@@ -11390,7 +11358,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="102" t="s">
+      <c r="A24" s="100" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="63">
@@ -11428,7 +11396,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="103"/>
+      <c r="A25" s="101"/>
       <c r="B25" s="63">
         <v>7</v>
       </c>
@@ -11464,7 +11432,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="104"/>
+      <c r="A26" s="102"/>
       <c r="B26" s="63">
         <v>5</v>
       </c>
@@ -12594,16 +12562,16 @@
       <c r="A1" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="103" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="105"/>
-      <c r="D1" s="99"/>
-      <c r="J1" s="98" t="s">
+      <c r="C1" s="104"/>
+      <c r="D1" s="105"/>
+      <c r="J1" s="103" t="s">
         <v>124</v>
       </c>
-      <c r="K1" s="105"/>
-      <c r="L1" s="99"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="105"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="74" t="s">

</xml_diff>

<commit_message>
Remove all unnecessary calculations from Stat block
</commit_message>
<xml_diff>
--- a/Tallaght Tallght Model_Original/control.xlsx
+++ b/Tallaght Tallght Model_Original/control.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sim Runs (2)" sheetId="33" r:id="rId1"/>
-    <sheet name="Zone1" sheetId="1" r:id="rId2"/>
+    <sheet name="Zone1" sheetId="1" state="hidden" r:id="rId2"/>
     <sheet name="Resus" sheetId="21" r:id="rId3"/>
     <sheet name="ZONE (1) MAJOR" sheetId="23" r:id="rId4"/>
     <sheet name="Zone2" sheetId="2" state="hidden" r:id="rId5"/>
@@ -1620,9 +1620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:Q1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2142,9 +2140,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2300,11 +2296,9 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2312,7 +2306,7 @@
     <col min="2" max="16384" width="8.88671875" style="48"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="83" t="s">
         <v>69</v>
       </c>
@@ -2320,261 +2314,147 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="84">
         <v>1</v>
       </c>
-      <c r="D2" s="84">
-        <v>1</v>
-      </c>
-      <c r="F2" s="84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="84">
         <v>7</v>
       </c>
-      <c r="D3" s="84">
-        <v>7</v>
-      </c>
-      <c r="F3" s="84">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="84">
         <v>10</v>
       </c>
-      <c r="D4" s="84">
-        <v>10</v>
-      </c>
-      <c r="F4" s="84">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="84">
         <v>8</v>
       </c>
-      <c r="D5" s="84">
-        <v>11</v>
-      </c>
-      <c r="F5" s="84">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="84">
         <v>3</v>
       </c>
-      <c r="C6" s="48">
-        <v>3</v>
-      </c>
-      <c r="D6" s="84">
-        <v>3</v>
-      </c>
-      <c r="F6" s="84">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="84">
         <v>4</v>
       </c>
-      <c r="D7" s="84">
-        <v>4</v>
-      </c>
-      <c r="F7" s="84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="84">
         <v>14</v>
       </c>
-      <c r="D8" s="84">
-        <v>36</v>
-      </c>
-      <c r="F8" s="84">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="84">
         <v>100</v>
       </c>
-      <c r="D9" s="84">
-        <v>100</v>
-      </c>
-      <c r="F9" s="84">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="58" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="84">
         <v>4</v>
       </c>
-      <c r="C10" s="48">
-        <v>1</v>
-      </c>
-      <c r="D10" s="84">
-        <v>1</v>
-      </c>
-      <c r="F10" s="84">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="58" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="84">
         <v>23</v>
       </c>
-      <c r="D11" s="84">
-        <v>23</v>
-      </c>
-      <c r="F11" s="84">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="84">
         <v>2</v>
       </c>
-      <c r="D12" s="84">
-        <v>1</v>
-      </c>
-      <c r="F12" s="84">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="58" t="s">
         <v>96</v>
       </c>
       <c r="B13" s="84">
         <v>10</v>
       </c>
-      <c r="D13" s="84">
-        <v>1</v>
-      </c>
-      <c r="F13" s="84">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="58" t="s">
         <v>97</v>
       </c>
       <c r="B14" s="84">
         <v>10</v>
       </c>
-      <c r="D14" s="84">
-        <v>1</v>
-      </c>
-      <c r="F14" s="84">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="58" t="s">
         <v>67</v>
       </c>
       <c r="B15" s="84">
         <v>100</v>
       </c>
-      <c r="D15" s="84">
-        <v>10</v>
-      </c>
-      <c r="F15" s="84">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="58" t="s">
         <v>95</v>
       </c>
       <c r="B16" s="84">
         <v>5</v>
       </c>
-      <c r="D16" s="84">
-        <v>3</v>
-      </c>
-      <c r="F16" s="84">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
         <v>99</v>
       </c>
       <c r="B17" s="84">
         <v>10</v>
       </c>
-      <c r="D17" s="84">
-        <v>2</v>
-      </c>
-      <c r="F17" s="84">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="58" t="s">
         <v>71</v>
       </c>
       <c r="B18" s="84">
         <v>7</v>
       </c>
-      <c r="D18" s="84">
-        <v>7</v>
-      </c>
-      <c r="F18" s="84">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="58" t="s">
         <v>98</v>
       </c>
       <c r="B19" s="84">
-        <v>10</v>
-      </c>
-      <c r="D19" s="84">
-        <v>2</v>
-      </c>
-      <c r="F19" s="84">
         <v>10</v>
       </c>
     </row>
@@ -2591,9 +2471,7 @@
   </sheetPr>
   <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2841,9 +2719,7 @@
   </sheetPr>
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3227,9 +3103,7 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3654,9 +3528,7 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4339,9 +4211,7 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5651,9 +5521,7 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7375,9 +7243,7 @@
   </sheetPr>
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8420,9 +8286,7 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8843,9 +8707,7 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10775,7 +10637,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -11520,7 +11382,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -12581,9 +12443,7 @@
   </sheetPr>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Add processes to AMAU & Triage blocks
- Add the "Approval" block to "Triage"
- Add processes of Blodd & ECG to "Prepare" block
- Organize the processes in AMAU as agreed in VSM & process map
</commit_message>
<xml_diff>
--- a/Tallaght Tallght Model_Original/control.xlsx
+++ b/Tallaght Tallght Model_Original/control.xlsx
@@ -1651,60 +1651,60 @@
         <v>143</v>
       </c>
       <c r="B1" s="37">
-        <v>4.4583599872227442</v>
+        <v>9.4736057574784471</v>
       </c>
       <c r="C1" s="37">
-        <v>9.8183659296948456</v>
+        <v>19.456779535111586</v>
       </c>
       <c r="D1" s="37">
-        <v>2.9269297179450011</v>
+        <v>7.1371182776068629</v>
       </c>
       <c r="E1" s="37">
-        <v>5.4764344229865012</v>
+        <v>12.229499457277424</v>
       </c>
       <c r="F1" s="37">
-        <v>9.8440354344834908</v>
+        <v>19.123833141007431</v>
       </c>
       <c r="G1" s="37">
-        <v>3.8021873685793248</v>
+        <v>10.208159769155204</v>
       </c>
       <c r="H1" s="37">
-        <v>3.4082678199301881</v>
+        <v>4.1657701993826768</v>
       </c>
       <c r="I1" s="37">
-        <v>3.6050104842361179</v>
+        <v>4.2327533637123578</v>
       </c>
       <c r="J1" s="37">
-        <v>3.2115251556242583</v>
+        <v>4.0876231743313838</v>
       </c>
       <c r="K1" s="38">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L1" s="38">
-        <v>115</v>
+        <v>1380</v>
       </c>
       <c r="M1" s="38">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N1" s="39">
-        <v>3.1668380006871057</v>
+        <v>16.270053665197519</v>
       </c>
       <c r="O1" s="39">
-        <v>0.81520040448645337</v>
+        <v>0.13187063212815422</v>
       </c>
       <c r="P1" s="39">
-        <v>0.38225894043642089</v>
+        <v>2.1661239725989826E-2</v>
       </c>
       <c r="Q1" s="39">
-        <v>46.731286907145062</v>
+        <v>39.630738559932787</v>
       </c>
       <c r="R1" s="40">
         <f>K1/L1</f>
-        <v>0.16521739130434782</v>
+        <v>1.7391304347826087E-2</v>
       </c>
       <c r="S1" s="40">
         <f>M1/K1</f>
-        <v>0.42105263157894735</v>
+        <v>0.29166666666666669</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -1968,67 +1968,67 @@
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B13" s="44">
         <f t="shared" ref="B13:L13" si="2">AVERAGE(B1:B10)</f>
-        <v>4.4583599872227442</v>
+        <v>9.4736057574784471</v>
       </c>
       <c r="C13" s="44">
         <f t="shared" si="2"/>
-        <v>9.8183659296948456</v>
+        <v>19.456779535111586</v>
       </c>
       <c r="D13" s="44">
         <f t="shared" si="2"/>
-        <v>2.9269297179450011</v>
+        <v>7.1371182776068629</v>
       </c>
       <c r="E13" s="44">
         <f t="shared" si="2"/>
-        <v>5.4764344229865012</v>
+        <v>12.229499457277424</v>
       </c>
       <c r="F13" s="44">
         <f t="shared" si="2"/>
-        <v>9.8440354344834908</v>
+        <v>19.123833141007431</v>
       </c>
       <c r="G13" s="44">
         <f t="shared" si="2"/>
-        <v>3.8021873685793248</v>
+        <v>10.208159769155204</v>
       </c>
       <c r="H13" s="44">
         <f t="shared" si="2"/>
-        <v>3.4082678199301881</v>
+        <v>4.1657701993826768</v>
       </c>
       <c r="I13" s="44">
         <f t="shared" si="2"/>
-        <v>3.6050104842361179</v>
+        <v>4.2327533637123578</v>
       </c>
       <c r="J13" s="44">
         <f t="shared" si="2"/>
-        <v>3.2115251556242583</v>
+        <v>4.0876231743313838</v>
       </c>
       <c r="K13" s="44">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L13" s="44">
         <f t="shared" si="2"/>
-        <v>115</v>
+        <v>1380</v>
       </c>
       <c r="M13" s="44">
         <f t="shared" ref="M13:S13" si="3">AVERAGE(M1:M10)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N13" s="44">
         <f t="shared" si="3"/>
-        <v>3.1668380006871057</v>
+        <v>16.270053665197519</v>
       </c>
       <c r="O13" s="44">
         <f t="shared" si="3"/>
-        <v>0.81520040448645337</v>
+        <v>0.13187063212815422</v>
       </c>
       <c r="P13" s="44">
         <f t="shared" si="3"/>
-        <v>0.38225894043642089</v>
+        <v>2.1661239725989826E-2</v>
       </c>
       <c r="Q13" s="44">
         <f t="shared" si="3"/>
-        <v>46.731286907145062</v>
+        <v>39.630738559932787</v>
       </c>
       <c r="R13" s="44" t="e">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Remove unnecessary hierarchies in AMAU
</commit_message>
<xml_diff>
--- a/Tallaght Tallght Model_Original/control.xlsx
+++ b/Tallaght Tallght Model_Original/control.xlsx
@@ -1651,60 +1651,60 @@
         <v>143</v>
       </c>
       <c r="B1" s="37">
-        <v>9.4736057574784471</v>
+        <v>7.8548539758837528</v>
       </c>
       <c r="C1" s="37">
-        <v>19.456779535111586</v>
+        <v>14.819505825125047</v>
       </c>
       <c r="D1" s="37">
-        <v>7.1371182776068629</v>
+        <v>6.0762197876987472</v>
       </c>
       <c r="E1" s="37">
-        <v>12.229499457277424</v>
+        <v>9.9591064651170917</v>
       </c>
       <c r="F1" s="37">
-        <v>19.123833141007431</v>
+        <v>15.725214051100446</v>
       </c>
       <c r="G1" s="37">
-        <v>10.208159769155204</v>
+        <v>8.006412362379157</v>
       </c>
       <c r="H1" s="37">
-        <v>4.1657701993826768</v>
+        <v>5.6957430509501119</v>
       </c>
       <c r="I1" s="37">
-        <v>4.2327533637123578</v>
+        <v>5.9705266151515977</v>
       </c>
       <c r="J1" s="37">
-        <v>4.0876231743313838</v>
+        <v>5.403373338639736</v>
       </c>
       <c r="K1" s="38">
-        <v>24</v>
+        <v>258</v>
       </c>
       <c r="L1" s="38">
         <v>1380</v>
       </c>
       <c r="M1" s="38">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="N1" s="39">
-        <v>16.270053665197519</v>
+        <v>77.516614696715607</v>
       </c>
       <c r="O1" s="39">
-        <v>0.13187063212815422</v>
+        <v>0.81189348123287064</v>
       </c>
       <c r="P1" s="39">
-        <v>2.1661239725989826E-2</v>
+        <v>0.35014700259657378</v>
       </c>
       <c r="Q1" s="39">
-        <v>39.630738559932787</v>
+        <v>58.646956703731725</v>
       </c>
       <c r="R1" s="40">
         <f>K1/L1</f>
-        <v>1.7391304347826087E-2</v>
+        <v>0.18695652173913044</v>
       </c>
       <c r="S1" s="40">
         <f>M1/K1</f>
-        <v>0.29166666666666669</v>
+        <v>0.20930232558139536</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -1968,43 +1968,43 @@
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B13" s="44">
         <f t="shared" ref="B13:L13" si="2">AVERAGE(B1:B10)</f>
-        <v>9.4736057574784471</v>
+        <v>7.8548539758837528</v>
       </c>
       <c r="C13" s="44">
         <f t="shared" si="2"/>
-        <v>19.456779535111586</v>
+        <v>14.819505825125047</v>
       </c>
       <c r="D13" s="44">
         <f t="shared" si="2"/>
-        <v>7.1371182776068629</v>
+        <v>6.0762197876987472</v>
       </c>
       <c r="E13" s="44">
         <f t="shared" si="2"/>
-        <v>12.229499457277424</v>
+        <v>9.9591064651170917</v>
       </c>
       <c r="F13" s="44">
         <f t="shared" si="2"/>
-        <v>19.123833141007431</v>
+        <v>15.725214051100446</v>
       </c>
       <c r="G13" s="44">
         <f t="shared" si="2"/>
-        <v>10.208159769155204</v>
+        <v>8.006412362379157</v>
       </c>
       <c r="H13" s="44">
         <f t="shared" si="2"/>
-        <v>4.1657701993826768</v>
+        <v>5.6957430509501119</v>
       </c>
       <c r="I13" s="44">
         <f t="shared" si="2"/>
-        <v>4.2327533637123578</v>
+        <v>5.9705266151515977</v>
       </c>
       <c r="J13" s="44">
         <f t="shared" si="2"/>
-        <v>4.0876231743313838</v>
+        <v>5.403373338639736</v>
       </c>
       <c r="K13" s="44">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>258</v>
       </c>
       <c r="L13" s="44">
         <f t="shared" si="2"/>
@@ -2012,23 +2012,23 @@
       </c>
       <c r="M13" s="44">
         <f t="shared" ref="M13:S13" si="3">AVERAGE(M1:M10)</f>
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="N13" s="44">
         <f t="shared" si="3"/>
-        <v>16.270053665197519</v>
+        <v>77.516614696715607</v>
       </c>
       <c r="O13" s="44">
         <f t="shared" si="3"/>
-        <v>0.13187063212815422</v>
+        <v>0.81189348123287064</v>
       </c>
       <c r="P13" s="44">
         <f t="shared" si="3"/>
-        <v>2.1661239725989826E-2</v>
+        <v>0.35014700259657378</v>
       </c>
       <c r="Q13" s="44">
         <f t="shared" si="3"/>
-        <v>39.630738559932787</v>
+        <v>58.646956703731725</v>
       </c>
       <c r="R13" s="44" t="e">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Changes in AMAU Process
1- Add porters to transfer block
2- Remove normal queues from all blocks in AMAU
3- Reneges patients in approval and transfer blocks in triage
4- Put a nurse in prepare block instead of SHO & a nurse
5- Put Registrar or SHO in interview step instead of a nurse
</commit_message>
<xml_diff>
--- a/Tallaght Tallght Model_Original/control.xlsx
+++ b/Tallaght Tallght Model_Original/control.xlsx
@@ -1651,34 +1651,34 @@
         <v>143</v>
       </c>
       <c r="B1" s="37">
-        <v>7.8548539758837528</v>
+        <v>7.908209390810466</v>
       </c>
       <c r="C1" s="37">
-        <v>14.819505825125047</v>
+        <v>15.220704057662301</v>
       </c>
       <c r="D1" s="37">
-        <v>6.0762197876987472</v>
+        <v>5.968808631341064</v>
       </c>
       <c r="E1" s="37">
-        <v>9.9591064651170917</v>
+        <v>9.9017630421611749</v>
       </c>
       <c r="F1" s="37">
-        <v>15.725214051100446</v>
+        <v>15.342493805003349</v>
       </c>
       <c r="G1" s="37">
-        <v>8.006412362379157</v>
+        <v>8.0970653227851361</v>
       </c>
       <c r="H1" s="37">
-        <v>5.6957430509501119</v>
+        <v>5.6266532508862817</v>
       </c>
       <c r="I1" s="37">
-        <v>5.9705266151515977</v>
+        <v>5.7817817238760387</v>
       </c>
       <c r="J1" s="37">
-        <v>5.403373338639736</v>
+        <v>5.4558515815297168</v>
       </c>
       <c r="K1" s="38">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="L1" s="38">
         <v>1380</v>
@@ -1687,24 +1687,24 @@
         <v>54</v>
       </c>
       <c r="N1" s="39">
-        <v>77.516614696715607</v>
+        <v>77.445168047473601</v>
       </c>
       <c r="O1" s="39">
-        <v>0.81189348123287064</v>
+        <v>0.80858076049480587</v>
       </c>
       <c r="P1" s="39">
-        <v>0.35014700259657378</v>
+        <v>0.45840945409760864</v>
       </c>
       <c r="Q1" s="39">
-        <v>58.646956703731725</v>
+        <v>51.957593278994821</v>
       </c>
       <c r="R1" s="40">
         <f>K1/L1</f>
-        <v>0.18695652173913044</v>
+        <v>0.19130434782608696</v>
       </c>
       <c r="S1" s="40">
         <f>M1/K1</f>
-        <v>0.20930232558139536</v>
+        <v>0.20454545454545456</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -1968,43 +1968,43 @@
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B13" s="44">
         <f t="shared" ref="B13:L13" si="2">AVERAGE(B1:B10)</f>
-        <v>7.8548539758837528</v>
+        <v>7.908209390810466</v>
       </c>
       <c r="C13" s="44">
         <f t="shared" si="2"/>
-        <v>14.819505825125047</v>
+        <v>15.220704057662301</v>
       </c>
       <c r="D13" s="44">
         <f t="shared" si="2"/>
-        <v>6.0762197876987472</v>
+        <v>5.968808631341064</v>
       </c>
       <c r="E13" s="44">
         <f t="shared" si="2"/>
-        <v>9.9591064651170917</v>
+        <v>9.9017630421611749</v>
       </c>
       <c r="F13" s="44">
         <f t="shared" si="2"/>
-        <v>15.725214051100446</v>
+        <v>15.342493805003349</v>
       </c>
       <c r="G13" s="44">
         <f t="shared" si="2"/>
-        <v>8.006412362379157</v>
+        <v>8.0970653227851361</v>
       </c>
       <c r="H13" s="44">
         <f t="shared" si="2"/>
-        <v>5.6957430509501119</v>
+        <v>5.6266532508862817</v>
       </c>
       <c r="I13" s="44">
         <f t="shared" si="2"/>
-        <v>5.9705266151515977</v>
+        <v>5.7817817238760387</v>
       </c>
       <c r="J13" s="44">
         <f t="shared" si="2"/>
-        <v>5.403373338639736</v>
+        <v>5.4558515815297168</v>
       </c>
       <c r="K13" s="44">
         <f t="shared" si="2"/>
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="L13" s="44">
         <f t="shared" si="2"/>
@@ -2016,19 +2016,19 @@
       </c>
       <c r="N13" s="44">
         <f t="shared" si="3"/>
-        <v>77.516614696715607</v>
+        <v>77.445168047473601</v>
       </c>
       <c r="O13" s="44">
         <f t="shared" si="3"/>
-        <v>0.81189348123287064</v>
+        <v>0.80858076049480587</v>
       </c>
       <c r="P13" s="44">
         <f t="shared" si="3"/>
-        <v>0.35014700259657378</v>
+        <v>0.45840945409760864</v>
       </c>
       <c r="Q13" s="44">
         <f t="shared" si="3"/>
-        <v>58.646956703731725</v>
+        <v>51.957593278994821</v>
       </c>
       <c r="R13" s="44" t="e">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Attempts to add reports to be sent to consultant
</commit_message>
<xml_diff>
--- a/Tallaght Tallght Model_Original/control.xlsx
+++ b/Tallaght Tallght Model_Original/control.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6396" tabRatio="843" firstSheet="10" activeTab="22"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6396" tabRatio="843"/>
   </bookViews>
   <sheets>
     <sheet name="Sim Runs (2)" sheetId="33" r:id="rId1"/>
@@ -1607,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -8403,7 +8403,7 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Delay discharge + LOS in AMU
- Delay discharge added to patients going to home, AMU & admitted
- PET in AMU changed according to distribution from real data
- Change time of blood tests & ECG
</commit_message>
<xml_diff>
--- a/Tallaght Tallght Model_Original/control.xlsx
+++ b/Tallaght Tallght Model_Original/control.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="155">
   <si>
     <t>Resources/Process</t>
   </si>
@@ -518,6 +518,21 @@
   </si>
   <si>
     <t>Board</t>
+  </si>
+  <si>
+    <t>LOS_AMU</t>
+  </si>
+  <si>
+    <t>Delay_Discharge_Home</t>
+  </si>
+  <si>
+    <t>Should be 1</t>
+  </si>
+  <si>
+    <t>Delay_Discharge_AMU</t>
+  </si>
+  <si>
+    <t>Delay_Discharge_Admit</t>
   </si>
 </sst>
 </file>
@@ -1608,7 +1623,7 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1640,60 +1655,60 @@
         <v>139</v>
       </c>
       <c r="B1" s="37">
-        <v>10.182479605394718</v>
+        <v>10.099403356786008</v>
       </c>
       <c r="C1" s="37">
-        <v>16.723852743722311</v>
+        <v>16.339253230175622</v>
       </c>
       <c r="D1" s="37">
-        <v>8.6751965060141067</v>
+        <v>8.5494866449044764</v>
       </c>
       <c r="E1" s="37">
-        <v>11.654920157426707</v>
+        <v>11.495546650319461</v>
       </c>
       <c r="F1" s="37">
-        <v>15.432080391909578</v>
+        <v>15.449903243702567</v>
       </c>
       <c r="G1" s="37">
-        <v>9.7509013006474508</v>
+        <v>9.7136591398322363</v>
       </c>
       <c r="H1" s="37">
-        <v>8.8314734312540484</v>
+        <v>8.9191100265415493</v>
       </c>
       <c r="I1" s="37">
-        <v>7.5711449165167357</v>
+        <v>8.8660778023630193</v>
       </c>
       <c r="J1" s="37">
-        <v>9.9674404065268121</v>
+        <v>8.9521782517376014</v>
       </c>
       <c r="K1" s="38">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="L1" s="38">
         <v>876</v>
       </c>
       <c r="M1" s="38">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="N1" s="39">
-        <v>78.582416899308711</v>
+        <v>0.15788551436337953</v>
       </c>
       <c r="O1" s="39">
-        <v>0.70025083694110013</v>
+        <v>0.700097409101615</v>
       </c>
       <c r="P1" s="39">
-        <v>0.43875399847568658</v>
+        <v>0.44083727952070501</v>
       </c>
       <c r="Q1" s="39">
-        <v>49.512229926717481</v>
+        <v>39.018415069798088</v>
       </c>
       <c r="R1" s="40">
         <f>K1/L1</f>
-        <v>0.24771689497716895</v>
+        <v>0.23515981735159816</v>
       </c>
       <c r="S1" s="40">
         <f>M1/K1</f>
-        <v>0.24884792626728111</v>
+        <v>0.470873786407767</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -1957,43 +1972,43 @@
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B13" s="44">
         <f t="shared" ref="B13:L13" si="2">AVERAGE(B1:B10)</f>
-        <v>10.182479605394718</v>
+        <v>10.099403356786008</v>
       </c>
       <c r="C13" s="44">
         <f t="shared" si="2"/>
-        <v>16.723852743722311</v>
+        <v>16.339253230175622</v>
       </c>
       <c r="D13" s="44">
         <f t="shared" si="2"/>
-        <v>8.6751965060141067</v>
+        <v>8.5494866449044764</v>
       </c>
       <c r="E13" s="44">
         <f t="shared" si="2"/>
-        <v>11.654920157426707</v>
+        <v>11.495546650319461</v>
       </c>
       <c r="F13" s="44">
         <f t="shared" si="2"/>
-        <v>15.432080391909578</v>
+        <v>15.449903243702567</v>
       </c>
       <c r="G13" s="44">
         <f t="shared" si="2"/>
-        <v>9.7509013006474508</v>
+        <v>9.7136591398322363</v>
       </c>
       <c r="H13" s="44">
         <f t="shared" si="2"/>
-        <v>8.8314734312540484</v>
+        <v>8.9191100265415493</v>
       </c>
       <c r="I13" s="44">
         <f t="shared" si="2"/>
-        <v>7.5711449165167357</v>
+        <v>8.8660778023630193</v>
       </c>
       <c r="J13" s="44">
         <f t="shared" si="2"/>
-        <v>9.9674404065268121</v>
+        <v>8.9521782517376014</v>
       </c>
       <c r="K13" s="44">
         <f t="shared" si="2"/>
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="L13" s="44">
         <f t="shared" si="2"/>
@@ -2001,23 +2016,23 @@
       </c>
       <c r="M13" s="44">
         <f t="shared" ref="M13:S13" si="3">AVERAGE(M1:M10)</f>
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="N13" s="44">
         <f t="shared" si="3"/>
-        <v>78.582416899308711</v>
+        <v>0.15788551436337953</v>
       </c>
       <c r="O13" s="44">
         <f t="shared" si="3"/>
-        <v>0.70025083694110013</v>
+        <v>0.700097409101615</v>
       </c>
       <c r="P13" s="44">
         <f t="shared" si="3"/>
-        <v>0.43875399847568658</v>
+        <v>0.44083727952070501</v>
       </c>
       <c r="Q13" s="44">
         <f t="shared" si="3"/>
-        <v>49.512229926717481</v>
+        <v>39.018415069798088</v>
       </c>
       <c r="R13" s="44" t="e">
         <f t="shared" si="3"/>
@@ -2127,7 +2142,7 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2135,10 +2150,19 @@
   <cols>
     <col min="1" max="1" width="15.33203125" style="48" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.88671875" style="48" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="48"/>
+    <col min="3" max="5" width="8.88671875" style="48"/>
+    <col min="6" max="6" width="13.21875" style="48" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.77734375" style="48" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="48"/>
+    <col min="9" max="9" width="13.21875" style="48" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.88671875" style="48" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="48"/>
+    <col min="12" max="12" width="13.21875" style="48" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.88671875" style="48" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="48"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="66" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="71" t="s">
         <v>47</v>
       </c>
@@ -2147,8 +2171,26 @@
       </c>
       <c r="C1" s="99"/>
       <c r="D1" s="100"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="85" t="s">
+        <v>151</v>
+      </c>
+      <c r="I1" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="85" t="s">
+        <v>153</v>
+      </c>
+      <c r="L1" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="85" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
         <v>61</v>
       </c>
@@ -2161,8 +2203,26 @@
       <c r="D2" s="77">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="87" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="87" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="87" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="76" t="s">
         <v>62</v>
       </c>
@@ -2175,8 +2235,26 @@
       <c r="D3" s="77">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" s="76">
+        <v>5</v>
+      </c>
+      <c r="G3" s="88">
+        <v>0.6</v>
+      </c>
+      <c r="I3" s="76">
+        <v>5</v>
+      </c>
+      <c r="J3" s="88">
+        <v>0.16</v>
+      </c>
+      <c r="L3" s="76">
+        <v>5</v>
+      </c>
+      <c r="M3" s="88">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="76" t="s">
         <v>63</v>
       </c>
@@ -2189,8 +2267,26 @@
       <c r="D4" s="77">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" s="76">
+        <v>10</v>
+      </c>
+      <c r="G4" s="88">
+        <v>0.16</v>
+      </c>
+      <c r="I4" s="76">
+        <v>10</v>
+      </c>
+      <c r="J4" s="88">
+        <v>0.05</v>
+      </c>
+      <c r="L4" s="76">
+        <v>10</v>
+      </c>
+      <c r="M4" s="88">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="78" t="s">
         <v>92</v>
       </c>
@@ -2201,24 +2297,60 @@
         <v>5</v>
       </c>
       <c r="D5" s="77">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="F5" s="76">
+        <v>15</v>
+      </c>
+      <c r="G5" s="88">
+        <v>0.05</v>
+      </c>
+      <c r="I5" s="76">
+        <v>15</v>
+      </c>
+      <c r="J5" s="88">
+        <v>0.06</v>
+      </c>
+      <c r="L5" s="76">
+        <v>15</v>
+      </c>
+      <c r="M5" s="88">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="79" t="s">
         <v>93</v>
       </c>
       <c r="B6" s="77">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C6" s="77">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D6" s="77">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="F6" s="76">
+        <v>20</v>
+      </c>
+      <c r="G6" s="88">
+        <v>0.03</v>
+      </c>
+      <c r="I6" s="76">
+        <v>20</v>
+      </c>
+      <c r="J6" s="88">
+        <v>0.01</v>
+      </c>
+      <c r="L6" s="76">
+        <v>20</v>
+      </c>
+      <c r="M6" s="88">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="80" t="s">
         <v>94</v>
       </c>
@@ -2231,8 +2363,26 @@
       <c r="D7" s="77">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7" s="76">
+        <v>25</v>
+      </c>
+      <c r="G7" s="88">
+        <v>0.02</v>
+      </c>
+      <c r="I7" s="76">
+        <v>25</v>
+      </c>
+      <c r="J7" s="88">
+        <v>0.01</v>
+      </c>
+      <c r="L7" s="76">
+        <v>25</v>
+      </c>
+      <c r="M7" s="88">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="80" t="s">
         <v>95</v>
       </c>
@@ -2245,8 +2395,26 @@
       <c r="D8" s="77">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8" s="76">
+        <v>30</v>
+      </c>
+      <c r="G8" s="88">
+        <v>0.02</v>
+      </c>
+      <c r="I8" s="76">
+        <v>30</v>
+      </c>
+      <c r="J8" s="88">
+        <v>0.05</v>
+      </c>
+      <c r="L8" s="76">
+        <v>30</v>
+      </c>
+      <c r="M8" s="88">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="80" t="s">
         <v>96</v>
       </c>
@@ -2259,8 +2427,46 @@
       <c r="D9" s="77">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F9" s="76">
+        <v>35</v>
+      </c>
+      <c r="G9" s="88">
+        <v>0.01</v>
+      </c>
+      <c r="I9" s="76">
+        <v>35</v>
+      </c>
+      <c r="J9" s="88">
+        <v>0.02</v>
+      </c>
+      <c r="L9" s="76">
+        <v>35</v>
+      </c>
+      <c r="M9" s="88">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F10" s="76">
+        <v>40</v>
+      </c>
+      <c r="G10" s="88">
+        <v>0.01</v>
+      </c>
+      <c r="I10" s="76">
+        <v>45</v>
+      </c>
+      <c r="J10" s="88">
+        <v>0.04</v>
+      </c>
+      <c r="L10" s="76">
+        <v>40</v>
+      </c>
+      <c r="M10" s="88">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" s="48" t="s">
         <v>90</v>
       </c>
@@ -2269,6 +2475,231 @@
       </c>
       <c r="D11" s="48" t="s">
         <v>87</v>
+      </c>
+      <c r="F11" s="76">
+        <v>45</v>
+      </c>
+      <c r="G11" s="88">
+        <v>0.01</v>
+      </c>
+      <c r="I11" s="76">
+        <v>50</v>
+      </c>
+      <c r="J11" s="88">
+        <v>0.04</v>
+      </c>
+      <c r="L11" s="76">
+        <v>45</v>
+      </c>
+      <c r="M11" s="88">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F12" s="76">
+        <v>50</v>
+      </c>
+      <c r="G12" s="88">
+        <v>0.02</v>
+      </c>
+      <c r="I12" s="76">
+        <v>55</v>
+      </c>
+      <c r="J12" s="88">
+        <v>0.05</v>
+      </c>
+      <c r="L12" s="76">
+        <v>50</v>
+      </c>
+      <c r="M12" s="88">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F13" s="76">
+        <v>55</v>
+      </c>
+      <c r="G13" s="88">
+        <v>0.01</v>
+      </c>
+      <c r="I13" s="76">
+        <v>60</v>
+      </c>
+      <c r="J13" s="88">
+        <v>0.03</v>
+      </c>
+      <c r="L13" s="76">
+        <v>55</v>
+      </c>
+      <c r="M13" s="88">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F14" s="76">
+        <v>60</v>
+      </c>
+      <c r="G14" s="88">
+        <v>0.02</v>
+      </c>
+      <c r="I14" s="76">
+        <v>120</v>
+      </c>
+      <c r="J14" s="88">
+        <v>0.25</v>
+      </c>
+      <c r="L14" s="76">
+        <v>60</v>
+      </c>
+      <c r="M14" s="88">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F15" s="76">
+        <v>120</v>
+      </c>
+      <c r="G15" s="88">
+        <v>0.03</v>
+      </c>
+      <c r="I15" s="76">
+        <v>180</v>
+      </c>
+      <c r="J15" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="L15" s="76">
+        <v>120</v>
+      </c>
+      <c r="M15" s="88">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F16" s="76">
+        <v>180</v>
+      </c>
+      <c r="G16" s="88">
+        <v>0.01</v>
+      </c>
+      <c r="I16" s="76">
+        <v>240</v>
+      </c>
+      <c r="J16" s="88">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L16" s="76">
+        <v>180</v>
+      </c>
+      <c r="M16" s="88">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="17" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F17" s="76"/>
+      <c r="G17" s="88"/>
+      <c r="I17" s="76">
+        <v>300</v>
+      </c>
+      <c r="J17" s="88">
+        <v>0.05</v>
+      </c>
+      <c r="L17" s="76">
+        <v>240</v>
+      </c>
+      <c r="M17" s="88">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F18" s="76"/>
+      <c r="G18" s="88"/>
+      <c r="I18" s="76">
+        <v>360</v>
+      </c>
+      <c r="J18" s="88">
+        <v>0.01</v>
+      </c>
+      <c r="L18" s="76">
+        <v>300</v>
+      </c>
+      <c r="M18" s="88">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="19" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F19" s="76"/>
+      <c r="G19" s="88"/>
+      <c r="I19" s="76"/>
+      <c r="J19" s="88"/>
+      <c r="L19" s="76">
+        <v>360</v>
+      </c>
+      <c r="M19" s="88">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="20" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F20" s="76"/>
+      <c r="G20" s="88"/>
+      <c r="I20" s="76"/>
+      <c r="J20" s="88"/>
+      <c r="L20" s="76">
+        <v>420</v>
+      </c>
+      <c r="M20" s="88">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="21" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F21" s="76"/>
+      <c r="G21" s="88"/>
+      <c r="I21" s="76"/>
+      <c r="J21" s="88"/>
+      <c r="L21" s="76">
+        <v>480</v>
+      </c>
+      <c r="M21" s="88">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="22" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F22" s="76"/>
+      <c r="G22" s="88"/>
+      <c r="I22" s="76"/>
+      <c r="J22" s="88"/>
+      <c r="L22" s="76"/>
+      <c r="M22" s="88"/>
+    </row>
+    <row r="23" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F23" s="76"/>
+      <c r="G23" s="88"/>
+      <c r="I23" s="76"/>
+      <c r="J23" s="88"/>
+      <c r="L23" s="76"/>
+      <c r="M23" s="88"/>
+    </row>
+    <row r="24" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F24" s="86" t="s">
+        <v>152</v>
+      </c>
+      <c r="G24" s="90">
+        <f>SUM(G3:G23)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="I24" s="86" t="s">
+        <v>152</v>
+      </c>
+      <c r="J24" s="90">
+        <f>SUM(J3:J23)</f>
+        <v>1</v>
+      </c>
+      <c r="L24" s="86" t="s">
+        <v>152</v>
+      </c>
+      <c r="M24" s="90">
+        <f>SUM(M3:M23)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2669,7 +3100,9 @@
   </sheetPr>
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N32" sqref="N32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3053,7 +3486,9 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:H24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8401,10 +8836,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -8418,10 +8853,13 @@
     <col min="7" max="7" width="8.88671875" style="48"/>
     <col min="8" max="8" width="13.44140625" style="48" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.33203125" style="48" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="48"/>
+    <col min="10" max="10" width="8.88671875" style="48"/>
+    <col min="11" max="11" width="13.44140625" style="48" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.33203125" style="48" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="48"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
         <v>26</v>
       </c>
@@ -8443,8 +8881,14 @@
       <c r="I1" s="85" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="85" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
         <v>27</v>
       </c>
@@ -8466,8 +8910,14 @@
       <c r="I2" s="87" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="87" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="76">
         <v>0</v>
       </c>
@@ -8492,8 +8942,17 @@
       <c r="J3" s="48" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="76">
+        <v>1</v>
+      </c>
+      <c r="L3" s="88">
+        <v>0.05</v>
+      </c>
+      <c r="M3" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="76">
         <v>1</v>
       </c>
@@ -8518,8 +8977,17 @@
       <c r="J4" s="48" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="76">
+        <v>2</v>
+      </c>
+      <c r="L4" s="88">
+        <v>0.2</v>
+      </c>
+      <c r="M4" s="48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="76">
         <v>2</v>
       </c>
@@ -8544,8 +9012,17 @@
       <c r="J5" s="48" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="76">
+        <v>3</v>
+      </c>
+      <c r="L5" s="88">
+        <v>0.22</v>
+      </c>
+      <c r="M5" s="48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="76">
         <v>3</v>
       </c>
@@ -8565,8 +9042,17 @@
       <c r="J6" s="48" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="76">
+        <v>4</v>
+      </c>
+      <c r="L6" s="88">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M6" s="48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="76">
         <v>4</v>
       </c>
@@ -8579,8 +9065,17 @@
         <v>4</v>
       </c>
       <c r="I7" s="88"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="76">
+        <v>5</v>
+      </c>
+      <c r="L7" s="88">
+        <v>0.12</v>
+      </c>
+      <c r="M7" s="48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="76">
         <v>5</v>
       </c>
@@ -8593,8 +9088,17 @@
         <v>5</v>
       </c>
       <c r="I8" s="88"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="76">
+        <v>6</v>
+      </c>
+      <c r="L8" s="88">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M8" s="48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="76">
         <v>6</v>
       </c>
@@ -8607,8 +9111,17 @@
         <v>6</v>
       </c>
       <c r="I9" s="88"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="76">
+        <v>7</v>
+      </c>
+      <c r="L9" s="88">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M9" s="48">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="76">
         <v>7</v>
       </c>
@@ -8621,8 +9134,17 @@
         <v>7</v>
       </c>
       <c r="I10" s="88"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="76">
+        <v>8</v>
+      </c>
+      <c r="L10" s="88">
+        <v>0.04</v>
+      </c>
+      <c r="M10" s="48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="76">
         <v>8</v>
       </c>
@@ -8635,8 +9157,17 @@
         <v>8</v>
       </c>
       <c r="I11" s="88"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="76">
+        <v>9</v>
+      </c>
+      <c r="L11" s="88">
+        <v>0.02</v>
+      </c>
+      <c r="M11" s="48">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="76">
         <v>9</v>
       </c>
@@ -8649,8 +9180,17 @@
         <v>9</v>
       </c>
       <c r="I12" s="88"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="76">
+        <v>10</v>
+      </c>
+      <c r="L12" s="88">
+        <v>0.03</v>
+      </c>
+      <c r="M12" s="48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="76">
         <v>10</v>
       </c>
@@ -8663,8 +9203,17 @@
         <v>10</v>
       </c>
       <c r="I13" s="88"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="76">
+        <v>15</v>
+      </c>
+      <c r="L13" s="88">
+        <v>0.02</v>
+      </c>
+      <c r="M13" s="48">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="76">
         <v>11</v>
       </c>
@@ -8677,8 +9226,17 @@
         <v>11</v>
       </c>
       <c r="I14" s="88"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="76">
+        <v>25</v>
+      </c>
+      <c r="L14" s="88">
+        <v>0.02</v>
+      </c>
+      <c r="M14" s="48">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="76">
         <v>12</v>
       </c>
@@ -8691,8 +9249,10 @@
         <v>12</v>
       </c>
       <c r="I15" s="88"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="76"/>
+      <c r="L15" s="88"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="76">
         <v>13</v>
       </c>
@@ -8705,8 +9265,10 @@
         <v>13</v>
       </c>
       <c r="I16" s="88"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K16" s="76"/>
+      <c r="L16" s="88"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="76">
         <v>14</v>
       </c>
@@ -8719,8 +9281,10 @@
         <v>14</v>
       </c>
       <c r="I17" s="88"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K17" s="76"/>
+      <c r="L17" s="88"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="76">
         <v>15</v>
       </c>
@@ -8733,8 +9297,10 @@
         <v>15</v>
       </c>
       <c r="I18" s="88"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K18" s="76"/>
+      <c r="L18" s="88"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="76">
         <v>16</v>
       </c>
@@ -8747,8 +9313,10 @@
         <v>16</v>
       </c>
       <c r="I19" s="88"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K19" s="76"/>
+      <c r="L19" s="88"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="76">
         <v>17</v>
       </c>
@@ -8761,8 +9329,10 @@
         <v>17</v>
       </c>
       <c r="I20" s="88"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K20" s="76"/>
+      <c r="L20" s="88"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="76">
         <v>18</v>
       </c>
@@ -8775,8 +9345,10 @@
         <v>18</v>
       </c>
       <c r="I21" s="88"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K21" s="76"/>
+      <c r="L21" s="88"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="76">
         <v>19</v>
       </c>
@@ -8789,8 +9361,10 @@
         <v>19</v>
       </c>
       <c r="I22" s="88"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K22" s="76"/>
+      <c r="L22" s="88"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="76">
         <v>20</v>
       </c>
@@ -8803,8 +9377,10 @@
         <v>20</v>
       </c>
       <c r="I23" s="88"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K23" s="76"/>
+      <c r="L23" s="88"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="86" t="s">
         <v>36</v>
       </c>
@@ -8825,6 +9401,13 @@
       <c r="I24" s="90">
         <f>SUM(I3:I23)</f>
         <v>1</v>
+      </c>
+      <c r="K24" s="86" t="s">
+        <v>36</v>
+      </c>
+      <c r="L24" s="90">
+        <f>SUM(L3:L23)</f>
+        <v>1.0000000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -10747,7 +11330,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -11209,7 +11792,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="64">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D19" s="64">
         <v>10</v>
@@ -11245,23 +11828,15 @@
         <v>7</v>
       </c>
       <c r="C20" s="64">
-        <v>7</v>
-      </c>
-      <c r="D20" s="64">
-        <v>2</v>
-      </c>
-      <c r="E20" s="64">
-        <v>2</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
       <c r="F20" s="56">
         <v>30</v>
       </c>
-      <c r="G20" s="64">
-        <v>1</v>
-      </c>
-      <c r="H20" s="64">
-        <v>1</v>
-      </c>
+      <c r="G20" s="64"/>
+      <c r="H20" s="64"/>
       <c r="I20" s="64">
         <v>7</v>
       </c>
@@ -11281,23 +11856,15 @@
         <v>5</v>
       </c>
       <c r="C21" s="64">
-        <v>5</v>
-      </c>
-      <c r="D21" s="64">
-        <v>0</v>
-      </c>
-      <c r="E21" s="64">
-        <v>0</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
       <c r="F21" s="56">
         <v>30</v>
       </c>
-      <c r="G21" s="64">
-        <v>0</v>
-      </c>
-      <c r="H21" s="64">
-        <v>0</v>
-      </c>
+      <c r="G21" s="64"/>
+      <c r="H21" s="64"/>
       <c r="I21" s="64">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Changes suggested by Extendsim Consultant
- Model every patient as two entities, one for processes in AMAU, and
the other for tests
- Unbatch the patient before taking any resources, then batch him when
the results are ready using queue matching or match batch
</commit_message>
<xml_diff>
--- a/Tallaght Tallght Model_Original/control.xlsx
+++ b/Tallaght Tallght Model_Original/control.xlsx
@@ -1655,60 +1655,60 @@
         <v>139</v>
       </c>
       <c r="B1" s="37">
-        <v>10.099403356786008</v>
+        <v>10.074437123570366</v>
       </c>
       <c r="C1" s="37">
-        <v>16.339253230175622</v>
+        <v>16.792125140216296</v>
       </c>
       <c r="D1" s="37">
-        <v>8.5494866449044764</v>
+        <v>8.7592093556054529</v>
       </c>
       <c r="E1" s="37">
-        <v>11.495546650319461</v>
+        <v>12.391329003934509</v>
       </c>
       <c r="F1" s="37">
-        <v>15.449903243702567</v>
+        <v>17.088768627171888</v>
       </c>
       <c r="G1" s="37">
-        <v>9.7136591398322363</v>
+        <v>10.294800840589581</v>
       </c>
       <c r="H1" s="37">
-        <v>8.9191100265415493</v>
+        <v>27.618491974775679</v>
       </c>
       <c r="I1" s="37">
-        <v>8.8660778023630193</v>
+        <v>23.658956504228993</v>
       </c>
       <c r="J1" s="37">
-        <v>8.9521782517376014</v>
+        <v>30.777443531798781</v>
       </c>
       <c r="K1" s="38">
-        <v>206</v>
+        <v>11</v>
       </c>
       <c r="L1" s="38">
         <v>876</v>
       </c>
       <c r="M1" s="38">
-        <v>97</v>
+        <v>4</v>
       </c>
       <c r="N1" s="39">
-        <v>0.15788551436337953</v>
+        <v>5.1720024299374792E-2</v>
       </c>
       <c r="O1" s="39">
-        <v>0.700097409101615</v>
+        <v>0.11404542049142317</v>
       </c>
       <c r="P1" s="39">
-        <v>0.44083727952070501</v>
+        <v>2.7148629304764863E-2</v>
       </c>
       <c r="Q1" s="39">
-        <v>39.018415069798088</v>
+        <v>23.401052798076023</v>
       </c>
       <c r="R1" s="40">
         <f>K1/L1</f>
-        <v>0.23515981735159816</v>
+        <v>1.2557077625570776E-2</v>
       </c>
       <c r="S1" s="40">
         <f>M1/K1</f>
-        <v>0.470873786407767</v>
+        <v>0.36363636363636365</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -1972,43 +1972,43 @@
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B13" s="44">
         <f t="shared" ref="B13:L13" si="2">AVERAGE(B1:B10)</f>
-        <v>10.099403356786008</v>
+        <v>10.074437123570366</v>
       </c>
       <c r="C13" s="44">
         <f t="shared" si="2"/>
-        <v>16.339253230175622</v>
+        <v>16.792125140216296</v>
       </c>
       <c r="D13" s="44">
         <f t="shared" si="2"/>
-        <v>8.5494866449044764</v>
+        <v>8.7592093556054529</v>
       </c>
       <c r="E13" s="44">
         <f t="shared" si="2"/>
-        <v>11.495546650319461</v>
+        <v>12.391329003934509</v>
       </c>
       <c r="F13" s="44">
         <f t="shared" si="2"/>
-        <v>15.449903243702567</v>
+        <v>17.088768627171888</v>
       </c>
       <c r="G13" s="44">
         <f t="shared" si="2"/>
-        <v>9.7136591398322363</v>
+        <v>10.294800840589581</v>
       </c>
       <c r="H13" s="44">
         <f t="shared" si="2"/>
-        <v>8.9191100265415493</v>
+        <v>27.618491974775679</v>
       </c>
       <c r="I13" s="44">
         <f t="shared" si="2"/>
-        <v>8.8660778023630193</v>
+        <v>23.658956504228993</v>
       </c>
       <c r="J13" s="44">
         <f t="shared" si="2"/>
-        <v>8.9521782517376014</v>
+        <v>30.777443531798781</v>
       </c>
       <c r="K13" s="44">
         <f t="shared" si="2"/>
-        <v>206</v>
+        <v>11</v>
       </c>
       <c r="L13" s="44">
         <f t="shared" si="2"/>
@@ -2016,23 +2016,23 @@
       </c>
       <c r="M13" s="44">
         <f t="shared" ref="M13:S13" si="3">AVERAGE(M1:M10)</f>
-        <v>97</v>
+        <v>4</v>
       </c>
       <c r="N13" s="44">
         <f t="shared" si="3"/>
-        <v>0.15788551436337953</v>
+        <v>5.1720024299374792E-2</v>
       </c>
       <c r="O13" s="44">
         <f t="shared" si="3"/>
-        <v>0.700097409101615</v>
+        <v>0.11404542049142317</v>
       </c>
       <c r="P13" s="44">
         <f t="shared" si="3"/>
-        <v>0.44083727952070501</v>
+        <v>2.7148629304764863E-2</v>
       </c>
       <c r="Q13" s="44">
         <f t="shared" si="3"/>
-        <v>39.018415069798088</v>
+        <v>23.401052798076023</v>
       </c>
       <c r="R13" s="44" t="e">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Attempts to make pts wait for blood results
- Add queue equation block in "consult" block, to make patients wait
based on a time assigned to one of their attributes
- This attribute was set in the "preparation" block, as a random number
</commit_message>
<xml_diff>
--- a/Tallaght Tallght Model_Original/control.xlsx
+++ b/Tallaght Tallght Model_Original/control.xlsx
@@ -1655,60 +1655,60 @@
         <v>139</v>
       </c>
       <c r="B1" s="37">
-        <v>10.074437123570366</v>
+        <v>10.14218928372175</v>
       </c>
       <c r="C1" s="37">
-        <v>16.792125140216296</v>
+        <v>16.10607236744913</v>
       </c>
       <c r="D1" s="37">
-        <v>8.7592093556054529</v>
+        <v>8.7513381471356162</v>
       </c>
       <c r="E1" s="37">
-        <v>12.391329003934509</v>
+        <v>11.768782637501435</v>
       </c>
       <c r="F1" s="37">
-        <v>17.088768627171888</v>
+        <v>16.194378879382157</v>
       </c>
       <c r="G1" s="37">
-        <v>10.294800840589581</v>
+        <v>9.6848497957387174</v>
       </c>
       <c r="H1" s="37">
-        <v>27.618491974775679</v>
+        <v>8.3534431851547239</v>
       </c>
       <c r="I1" s="37">
-        <v>23.658956504228993</v>
+        <v>9.1269643916629288</v>
       </c>
       <c r="J1" s="37">
-        <v>30.777443531798781</v>
+        <v>7.6855968015611849</v>
       </c>
       <c r="K1" s="38">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="L1" s="38">
         <v>876</v>
       </c>
       <c r="M1" s="38">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="N1" s="39">
-        <v>5.1720024299374792E-2</v>
+        <v>4.4604828359562698E-2</v>
       </c>
       <c r="O1" s="39">
-        <v>0.11404542049142317</v>
+        <v>0.49592987168692232</v>
       </c>
       <c r="P1" s="39">
-        <v>2.7148629304764863E-2</v>
+        <v>0.2938976159510695</v>
       </c>
       <c r="Q1" s="39">
-        <v>23.401052798076023</v>
+        <v>28.035741637538155</v>
       </c>
       <c r="R1" s="40">
         <f>K1/L1</f>
-        <v>1.2557077625570776E-2</v>
+        <v>0.2180365296803653</v>
       </c>
       <c r="S1" s="40">
         <f>M1/K1</f>
-        <v>0.36363636363636365</v>
+        <v>0.14659685863874344</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -1972,43 +1972,43 @@
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B13" s="44">
         <f t="shared" ref="B13:L13" si="2">AVERAGE(B1:B10)</f>
-        <v>10.074437123570366</v>
+        <v>10.14218928372175</v>
       </c>
       <c r="C13" s="44">
         <f t="shared" si="2"/>
-        <v>16.792125140216296</v>
+        <v>16.10607236744913</v>
       </c>
       <c r="D13" s="44">
         <f t="shared" si="2"/>
-        <v>8.7592093556054529</v>
+        <v>8.7513381471356162</v>
       </c>
       <c r="E13" s="44">
         <f t="shared" si="2"/>
-        <v>12.391329003934509</v>
+        <v>11.768782637501435</v>
       </c>
       <c r="F13" s="44">
         <f t="shared" si="2"/>
-        <v>17.088768627171888</v>
+        <v>16.194378879382157</v>
       </c>
       <c r="G13" s="44">
         <f t="shared" si="2"/>
-        <v>10.294800840589581</v>
+        <v>9.6848497957387174</v>
       </c>
       <c r="H13" s="44">
         <f t="shared" si="2"/>
-        <v>27.618491974775679</v>
+        <v>8.3534431851547239</v>
       </c>
       <c r="I13" s="44">
         <f t="shared" si="2"/>
-        <v>23.658956504228993</v>
+        <v>9.1269643916629288</v>
       </c>
       <c r="J13" s="44">
         <f t="shared" si="2"/>
-        <v>30.777443531798781</v>
+        <v>7.6855968015611849</v>
       </c>
       <c r="K13" s="44">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="L13" s="44">
         <f t="shared" si="2"/>
@@ -2016,23 +2016,23 @@
       </c>
       <c r="M13" s="44">
         <f t="shared" ref="M13:S13" si="3">AVERAGE(M1:M10)</f>
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="N13" s="44">
         <f t="shared" si="3"/>
-        <v>5.1720024299374792E-2</v>
+        <v>4.4604828359562698E-2</v>
       </c>
       <c r="O13" s="44">
         <f t="shared" si="3"/>
-        <v>0.11404542049142317</v>
+        <v>0.49592987168692232</v>
       </c>
       <c r="P13" s="44">
         <f t="shared" si="3"/>
-        <v>2.7148629304764863E-2</v>
+        <v>0.2938976159510695</v>
       </c>
       <c r="Q13" s="44">
         <f t="shared" si="3"/>
-        <v>23.401052798076023</v>
+        <v>28.035741637538155</v>
       </c>
       <c r="R13" s="44" t="e">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Change mechanism of discharge from AMAU
- Pts are assigned an attribute in "Decision" block, either to be
admitted or discharged
- Based on that attribute, they get routed in "Out_Dist" block
- Pts to be admitted either get admitted to a ward, AMU, or if no bed
available, they board an AMAU bed. This is done based on the following
availability conditions:
- Based on ward availability, patients to be admitted to ward can either
get a bed directly or go to AMU if a bed is available
- Based on AMU availability, patients to be admitted to AMU can either
get a bed directly or board an AMAU bed
</commit_message>
<xml_diff>
--- a/Tallaght Tallght Model_Original/control.xlsx
+++ b/Tallaght Tallght Model_Original/control.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6396" tabRatio="843"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6396" tabRatio="843" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Sim Runs (2)" sheetId="33" r:id="rId1"/>
@@ -1622,7 +1622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
@@ -1655,60 +1655,60 @@
         <v>139</v>
       </c>
       <c r="B1" s="37">
-        <v>10.14218928372175</v>
+        <v>9.6765676999445098</v>
       </c>
       <c r="C1" s="37">
-        <v>16.10607236744913</v>
+        <v>15.497687865527437</v>
       </c>
       <c r="D1" s="37">
-        <v>8.7513381471356162</v>
+        <v>8.2714697289417565</v>
       </c>
       <c r="E1" s="37">
-        <v>11.768782637501435</v>
+        <v>11.305352564199476</v>
       </c>
       <c r="F1" s="37">
-        <v>16.194378879382157</v>
+        <v>15.498246797761322</v>
       </c>
       <c r="G1" s="37">
-        <v>9.6848497957387174</v>
+        <v>9.1897965466158702</v>
       </c>
       <c r="H1" s="37">
-        <v>8.3534431851547239</v>
+        <v>5.7006499367053944</v>
       </c>
       <c r="I1" s="37">
-        <v>9.1269643916629288</v>
+        <v>5.6275578193680547</v>
       </c>
       <c r="J1" s="37">
-        <v>7.6855968015611849</v>
+        <v>5.7725354861507547</v>
       </c>
       <c r="K1" s="38">
-        <v>191</v>
+        <v>249</v>
       </c>
       <c r="L1" s="38">
         <v>876</v>
       </c>
       <c r="M1" s="38">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="N1" s="39">
-        <v>4.4604828359562698E-2</v>
+        <v>2.4326264639408222</v>
       </c>
       <c r="O1" s="39">
-        <v>0.49592987168692232</v>
+        <v>0.57709758891276297</v>
       </c>
       <c r="P1" s="39">
-        <v>0.2938976159510695</v>
+        <v>0.58339396294076529</v>
       </c>
       <c r="Q1" s="39">
-        <v>28.035741637538155</v>
+        <v>36.374687944784924</v>
       </c>
       <c r="R1" s="40">
         <f>K1/L1</f>
-        <v>0.2180365296803653</v>
+        <v>0.28424657534246578</v>
       </c>
       <c r="S1" s="40">
         <f>M1/K1</f>
-        <v>0.14659685863874344</v>
+        <v>0.40562248995983935</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -1972,43 +1972,43 @@
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B13" s="44">
         <f t="shared" ref="B13:L13" si="2">AVERAGE(B1:B10)</f>
-        <v>10.14218928372175</v>
+        <v>9.6765676999445098</v>
       </c>
       <c r="C13" s="44">
         <f t="shared" si="2"/>
-        <v>16.10607236744913</v>
+        <v>15.497687865527437</v>
       </c>
       <c r="D13" s="44">
         <f t="shared" si="2"/>
-        <v>8.7513381471356162</v>
+        <v>8.2714697289417565</v>
       </c>
       <c r="E13" s="44">
         <f t="shared" si="2"/>
-        <v>11.768782637501435</v>
+        <v>11.305352564199476</v>
       </c>
       <c r="F13" s="44">
         <f t="shared" si="2"/>
-        <v>16.194378879382157</v>
+        <v>15.498246797761322</v>
       </c>
       <c r="G13" s="44">
         <f t="shared" si="2"/>
-        <v>9.6848497957387174</v>
+        <v>9.1897965466158702</v>
       </c>
       <c r="H13" s="44">
         <f t="shared" si="2"/>
-        <v>8.3534431851547239</v>
+        <v>5.7006499367053944</v>
       </c>
       <c r="I13" s="44">
         <f t="shared" si="2"/>
-        <v>9.1269643916629288</v>
+        <v>5.6275578193680547</v>
       </c>
       <c r="J13" s="44">
         <f t="shared" si="2"/>
-        <v>7.6855968015611849</v>
+        <v>5.7725354861507547</v>
       </c>
       <c r="K13" s="44">
         <f t="shared" si="2"/>
-        <v>191</v>
+        <v>249</v>
       </c>
       <c r="L13" s="44">
         <f t="shared" si="2"/>
@@ -2016,23 +2016,23 @@
       </c>
       <c r="M13" s="44">
         <f t="shared" ref="M13:S13" si="3">AVERAGE(M1:M10)</f>
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="N13" s="44">
         <f t="shared" si="3"/>
-        <v>4.4604828359562698E-2</v>
+        <v>2.4326264639408222</v>
       </c>
       <c r="O13" s="44">
         <f t="shared" si="3"/>
-        <v>0.49592987168692232</v>
+        <v>0.57709758891276297</v>
       </c>
       <c r="P13" s="44">
         <f t="shared" si="3"/>
-        <v>0.2938976159510695</v>
+        <v>0.58339396294076529</v>
       </c>
       <c r="Q13" s="44">
         <f t="shared" si="3"/>
-        <v>28.035741637538155</v>
+        <v>36.374687944784924</v>
       </c>
       <c r="R13" s="44" t="e">
         <f t="shared" si="3"/>
@@ -2891,7 +2891,9 @@
   </sheetPr>
   <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Add Delay to transfer block
Add a process to delay patients in transfer block, with a processing
time following a triag. dist. (min=10, avg=20, max=40)
</commit_message>
<xml_diff>
--- a/Tallaght Tallght Model_Original/control.xlsx
+++ b/Tallaght Tallght Model_Original/control.xlsx
@@ -1653,34 +1653,34 @@
         <v>139</v>
       </c>
       <c r="B1" s="37">
-        <v>9.9350577369051045</v>
+        <v>9.5750552440755552</v>
       </c>
       <c r="C1" s="37">
-        <v>16.097864540597552</v>
+        <v>15.446869887566738</v>
       </c>
       <c r="D1" s="37">
-        <v>8.471461216646933</v>
+        <v>8.2362393379294776</v>
       </c>
       <c r="E1" s="37">
-        <v>11.461329428488494</v>
+        <v>11.837756784200176</v>
       </c>
       <c r="F1" s="37">
-        <v>15.849224889545203</v>
+        <v>16.008961678729111</v>
       </c>
       <c r="G1" s="37">
-        <v>9.489988213202146</v>
+        <v>9.9067953114208951</v>
       </c>
       <c r="H1" s="37">
-        <v>3.1121181119842372</v>
+        <v>3.4235156480692246</v>
       </c>
       <c r="I1" s="37">
-        <v>2.9015048348979495</v>
+        <v>3.1309059271261939</v>
       </c>
       <c r="J1" s="37">
-        <v>3.3310504860295636</v>
+        <v>3.7810771683162132</v>
       </c>
       <c r="K1" s="38">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="L1" s="38">
         <v>876</v>
@@ -1689,24 +1689,24 @@
         <v>52</v>
       </c>
       <c r="N1" s="39">
-        <v>87.85740776603086</v>
+        <v>86.742501845115441</v>
       </c>
       <c r="O1" s="39">
-        <v>0.50189945092894894</v>
+        <v>0.47093225571622427</v>
       </c>
       <c r="P1" s="39">
-        <v>0.51330704086229584</v>
+        <v>0.47177992951933095</v>
       </c>
       <c r="Q1" s="39">
-        <v>22.927732909190425</v>
+        <v>21.357186228809375</v>
       </c>
       <c r="R1" s="40">
         <f>K1/L1</f>
-        <v>0.19748858447488585</v>
+        <v>0.18264840182648401</v>
       </c>
       <c r="S1" s="40">
         <f>M1/K1</f>
-        <v>0.30057803468208094</v>
+        <v>0.32500000000000001</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -1970,43 +1970,43 @@
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B13" s="44">
         <f t="shared" ref="B13:L13" si="2">AVERAGE(B1:B10)</f>
-        <v>9.9350577369051045</v>
+        <v>9.5750552440755552</v>
       </c>
       <c r="C13" s="44">
         <f t="shared" si="2"/>
-        <v>16.097864540597552</v>
+        <v>15.446869887566738</v>
       </c>
       <c r="D13" s="44">
         <f t="shared" si="2"/>
-        <v>8.471461216646933</v>
+        <v>8.2362393379294776</v>
       </c>
       <c r="E13" s="44">
         <f t="shared" si="2"/>
-        <v>11.461329428488494</v>
+        <v>11.837756784200176</v>
       </c>
       <c r="F13" s="44">
         <f t="shared" si="2"/>
-        <v>15.849224889545203</v>
+        <v>16.008961678729111</v>
       </c>
       <c r="G13" s="44">
         <f t="shared" si="2"/>
-        <v>9.489988213202146</v>
+        <v>9.9067953114208951</v>
       </c>
       <c r="H13" s="44">
         <f t="shared" si="2"/>
-        <v>3.1121181119842372</v>
+        <v>3.4235156480692246</v>
       </c>
       <c r="I13" s="44">
         <f t="shared" si="2"/>
-        <v>2.9015048348979495</v>
+        <v>3.1309059271261939</v>
       </c>
       <c r="J13" s="44">
         <f t="shared" si="2"/>
-        <v>3.3310504860295636</v>
+        <v>3.7810771683162132</v>
       </c>
       <c r="K13" s="44">
         <f t="shared" si="2"/>
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="L13" s="44">
         <f t="shared" si="2"/>
@@ -2018,19 +2018,19 @@
       </c>
       <c r="N13" s="44">
         <f t="shared" si="3"/>
-        <v>87.85740776603086</v>
+        <v>86.742501845115441</v>
       </c>
       <c r="O13" s="44">
         <f t="shared" si="3"/>
-        <v>0.50189945092894894</v>
+        <v>0.47093225571622427</v>
       </c>
       <c r="P13" s="44">
         <f t="shared" si="3"/>
-        <v>0.51330704086229584</v>
+        <v>0.47177992951933095</v>
       </c>
       <c r="Q13" s="44">
         <f t="shared" si="3"/>
-        <v>22.927732909190425</v>
+        <v>21.357186228809375</v>
       </c>
       <c r="R13" s="44" t="e">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Add boarders from ED to AMAU
Each working day in AMAU, patients are generated to board beds in AMAU
</commit_message>
<xml_diff>
--- a/Tallaght Tallght Model_Original/control.xlsx
+++ b/Tallaght Tallght Model_Original/control.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6396" tabRatio="843"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6396" tabRatio="843" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Sim Runs (2)" sheetId="33" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="153">
   <si>
     <t>Resources/Process</t>
   </si>
@@ -527,12 +527,6 @@
   </si>
   <si>
     <t>Should be 1</t>
-  </si>
-  <si>
-    <t>Delay_Discharge_AMU</t>
-  </si>
-  <si>
-    <t>Delay_Discharge_Admit</t>
   </si>
 </sst>
 </file>
@@ -1060,7 +1054,7 @@
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1310,6 +1304,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1622,7 +1622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1653,31 +1653,31 @@
         <v>139</v>
       </c>
       <c r="B1" s="37">
-        <v>9.5750552440755552</v>
+        <v>9.6442449082317303</v>
       </c>
       <c r="C1" s="37">
-        <v>15.446869887566738</v>
+        <v>16.024034709732955</v>
       </c>
       <c r="D1" s="37">
-        <v>8.2362393379294776</v>
+        <v>8.2067877806044223</v>
       </c>
       <c r="E1" s="37">
-        <v>11.837756784200176</v>
+        <v>11.907438265403261</v>
       </c>
       <c r="F1" s="37">
-        <v>16.008961678729111</v>
+        <v>15.547793926061498</v>
       </c>
       <c r="G1" s="37">
-        <v>9.9067953114208951</v>
+        <v>10.124476477365306</v>
       </c>
       <c r="H1" s="37">
-        <v>3.4235156480692246</v>
+        <v>3.4531053112230436</v>
       </c>
       <c r="I1" s="37">
-        <v>3.1309059271261939</v>
+        <v>3.2767801129094156</v>
       </c>
       <c r="J1" s="37">
-        <v>3.7810771683162132</v>
+        <v>3.685650137984497</v>
       </c>
       <c r="K1" s="38">
         <v>160</v>
@@ -1689,16 +1689,16 @@
         <v>52</v>
       </c>
       <c r="N1" s="39">
-        <v>86.742501845115441</v>
+        <v>87.192904652790475</v>
       </c>
       <c r="O1" s="39">
-        <v>0.47093225571622427</v>
+        <v>0.45867107344831592</v>
       </c>
       <c r="P1" s="39">
-        <v>0.47177992951933095</v>
+        <v>0.46471391752409263</v>
       </c>
       <c r="Q1" s="39">
-        <v>21.357186228809375</v>
+        <v>28.620095749056375</v>
       </c>
       <c r="R1" s="40">
         <f>K1/L1</f>
@@ -1970,39 +1970,39 @@
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B13" s="44">
         <f t="shared" ref="B13:L13" si="2">AVERAGE(B1:B10)</f>
-        <v>9.5750552440755552</v>
+        <v>9.6442449082317303</v>
       </c>
       <c r="C13" s="44">
         <f t="shared" si="2"/>
-        <v>15.446869887566738</v>
+        <v>16.024034709732955</v>
       </c>
       <c r="D13" s="44">
         <f t="shared" si="2"/>
-        <v>8.2362393379294776</v>
+        <v>8.2067877806044223</v>
       </c>
       <c r="E13" s="44">
         <f t="shared" si="2"/>
-        <v>11.837756784200176</v>
+        <v>11.907438265403261</v>
       </c>
       <c r="F13" s="44">
         <f t="shared" si="2"/>
-        <v>16.008961678729111</v>
+        <v>15.547793926061498</v>
       </c>
       <c r="G13" s="44">
         <f t="shared" si="2"/>
-        <v>9.9067953114208951</v>
+        <v>10.124476477365306</v>
       </c>
       <c r="H13" s="44">
         <f t="shared" si="2"/>
-        <v>3.4235156480692246</v>
+        <v>3.4531053112230436</v>
       </c>
       <c r="I13" s="44">
         <f t="shared" si="2"/>
-        <v>3.1309059271261939</v>
+        <v>3.2767801129094156</v>
       </c>
       <c r="J13" s="44">
         <f t="shared" si="2"/>
-        <v>3.7810771683162132</v>
+        <v>3.685650137984497</v>
       </c>
       <c r="K13" s="44">
         <f t="shared" si="2"/>
@@ -2018,19 +2018,19 @@
       </c>
       <c r="N13" s="44">
         <f t="shared" si="3"/>
-        <v>86.742501845115441</v>
+        <v>87.192904652790475</v>
       </c>
       <c r="O13" s="44">
         <f t="shared" si="3"/>
-        <v>0.47093225571622427</v>
+        <v>0.45867107344831592</v>
       </c>
       <c r="P13" s="44">
         <f t="shared" si="3"/>
-        <v>0.47177992951933095</v>
+        <v>0.46471391752409263</v>
       </c>
       <c r="Q13" s="44">
         <f t="shared" si="3"/>
-        <v>21.357186228809375</v>
+        <v>28.620095749056375</v>
       </c>
       <c r="R13" s="44" t="e">
         <f t="shared" si="3"/>
@@ -2140,7 +2140,7 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2151,16 +2151,10 @@
     <col min="3" max="5" width="8.88671875" style="48"/>
     <col min="6" max="6" width="13.21875" style="48" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.77734375" style="48" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="48"/>
-    <col min="9" max="9" width="13.21875" style="48" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.88671875" style="48" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="48"/>
-    <col min="12" max="12" width="13.21875" style="48" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.88671875" style="48" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="48"/>
+    <col min="8" max="16384" width="8.88671875" style="48"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="66" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="71" t="s">
         <v>47</v>
       </c>
@@ -2175,20 +2169,8 @@
       <c r="G1" s="85" t="s">
         <v>151</v>
       </c>
-      <c r="I1" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="85" t="s">
-        <v>153</v>
-      </c>
-      <c r="L1" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" s="85" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
         <v>61</v>
       </c>
@@ -2207,20 +2189,8 @@
       <c r="G2" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="87" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="87" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="76" t="s">
         <v>62</v>
       </c>
@@ -2233,26 +2203,14 @@
       <c r="D3" s="77">
         <v>15</v>
       </c>
-      <c r="F3" s="76">
+      <c r="F3" s="105">
         <v>5</v>
       </c>
-      <c r="G3" s="88">
+      <c r="G3" s="106">
         <v>0.6</v>
       </c>
-      <c r="I3" s="76">
-        <v>5</v>
-      </c>
-      <c r="J3" s="88">
-        <v>0.16</v>
-      </c>
-      <c r="L3" s="76">
-        <v>5</v>
-      </c>
-      <c r="M3" s="88">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="76" t="s">
         <v>63</v>
       </c>
@@ -2265,26 +2223,14 @@
       <c r="D4" s="77">
         <v>30</v>
       </c>
-      <c r="F4" s="76">
+      <c r="F4" s="105">
         <v>10</v>
       </c>
-      <c r="G4" s="88">
+      <c r="G4" s="106">
         <v>0.16</v>
       </c>
-      <c r="I4" s="76">
-        <v>10</v>
-      </c>
-      <c r="J4" s="88">
-        <v>0.05</v>
-      </c>
-      <c r="L4" s="76">
-        <v>10</v>
-      </c>
-      <c r="M4" s="88">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="78" t="s">
         <v>92</v>
       </c>
@@ -2297,26 +2243,14 @@
       <c r="D5" s="77">
         <v>20</v>
       </c>
-      <c r="F5" s="76">
+      <c r="F5" s="105">
         <v>15</v>
       </c>
-      <c r="G5" s="88">
+      <c r="G5" s="106">
         <v>0.05</v>
       </c>
-      <c r="I5" s="76">
-        <v>15</v>
-      </c>
-      <c r="J5" s="88">
-        <v>0.06</v>
-      </c>
-      <c r="L5" s="76">
-        <v>15</v>
-      </c>
-      <c r="M5" s="88">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="79" t="s">
         <v>93</v>
       </c>
@@ -2329,26 +2263,14 @@
       <c r="D6" s="77">
         <v>20</v>
       </c>
-      <c r="F6" s="76">
+      <c r="F6" s="105">
         <v>20</v>
       </c>
-      <c r="G6" s="88">
+      <c r="G6" s="106">
         <v>0.03</v>
       </c>
-      <c r="I6" s="76">
-        <v>20</v>
-      </c>
-      <c r="J6" s="88">
-        <v>0.01</v>
-      </c>
-      <c r="L6" s="76">
-        <v>20</v>
-      </c>
-      <c r="M6" s="88">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="80" t="s">
         <v>94</v>
       </c>
@@ -2361,26 +2283,14 @@
       <c r="D7" s="77">
         <v>40</v>
       </c>
-      <c r="F7" s="76">
+      <c r="F7" s="105">
         <v>25</v>
       </c>
-      <c r="G7" s="88">
+      <c r="G7" s="106">
         <v>0.02</v>
       </c>
-      <c r="I7" s="76">
-        <v>25</v>
-      </c>
-      <c r="J7" s="88">
-        <v>0.01</v>
-      </c>
-      <c r="L7" s="76">
-        <v>25</v>
-      </c>
-      <c r="M7" s="88">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="80" t="s">
         <v>95</v>
       </c>
@@ -2393,26 +2303,14 @@
       <c r="D8" s="77">
         <v>40</v>
       </c>
-      <c r="F8" s="76">
+      <c r="F8" s="105">
         <v>30</v>
       </c>
-      <c r="G8" s="88">
+      <c r="G8" s="106">
         <v>0.02</v>
       </c>
-      <c r="I8" s="76">
-        <v>30</v>
-      </c>
-      <c r="J8" s="88">
-        <v>0.05</v>
-      </c>
-      <c r="L8" s="76">
-        <v>30</v>
-      </c>
-      <c r="M8" s="88">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="80" t="s">
         <v>96</v>
       </c>
@@ -2425,46 +2323,22 @@
       <c r="D9" s="77">
         <v>40</v>
       </c>
-      <c r="F9" s="76">
+      <c r="F9" s="105">
         <v>35</v>
       </c>
-      <c r="G9" s="88">
+      <c r="G9" s="106">
         <v>0.01</v>
       </c>
-      <c r="I9" s="76">
-        <v>35</v>
-      </c>
-      <c r="J9" s="88">
-        <v>0.02</v>
-      </c>
-      <c r="L9" s="76">
-        <v>35</v>
-      </c>
-      <c r="M9" s="88">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F10" s="76">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F10" s="105">
         <v>40</v>
       </c>
-      <c r="G10" s="88">
+      <c r="G10" s="106">
         <v>0.01</v>
       </c>
-      <c r="I10" s="76">
-        <v>45</v>
-      </c>
-      <c r="J10" s="88">
-        <v>0.04</v>
-      </c>
-      <c r="L10" s="76">
-        <v>40</v>
-      </c>
-      <c r="M10" s="88">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="48" t="s">
         <v>90</v>
       </c>
@@ -2474,230 +2348,88 @@
       <c r="D11" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="F11" s="76">
+      <c r="F11" s="105">
         <v>45</v>
       </c>
-      <c r="G11" s="88">
+      <c r="G11" s="106">
         <v>0.01</v>
       </c>
-      <c r="I11" s="76">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F12" s="105">
         <v>50</v>
       </c>
-      <c r="J11" s="88">
-        <v>0.04</v>
-      </c>
-      <c r="L11" s="76">
-        <v>45</v>
-      </c>
-      <c r="M11" s="88">
+      <c r="G12" s="106">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F13" s="105">
+        <v>55</v>
+      </c>
+      <c r="G13" s="106">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F14" s="105">
+        <v>60</v>
+      </c>
+      <c r="G14" s="106">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F15" s="105">
+        <v>120</v>
+      </c>
+      <c r="G15" s="106">
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F12" s="76">
-        <v>50</v>
-      </c>
-      <c r="G12" s="88">
-        <v>0.02</v>
-      </c>
-      <c r="I12" s="76">
-        <v>55</v>
-      </c>
-      <c r="J12" s="88">
-        <v>0.05</v>
-      </c>
-      <c r="L12" s="76">
-        <v>50</v>
-      </c>
-      <c r="M12" s="88">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F13" s="76">
-        <v>55</v>
-      </c>
-      <c r="G13" s="88">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F16" s="105">
+        <v>180</v>
+      </c>
+      <c r="G16" s="106">
         <v>0.01</v>
       </c>
-      <c r="I13" s="76">
-        <v>60</v>
-      </c>
-      <c r="J13" s="88">
-        <v>0.03</v>
-      </c>
-      <c r="L13" s="76">
-        <v>55</v>
-      </c>
-      <c r="M13" s="88">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F14" s="76">
-        <v>60</v>
-      </c>
-      <c r="G14" s="88">
-        <v>0.02</v>
-      </c>
-      <c r="I14" s="76">
-        <v>120</v>
-      </c>
-      <c r="J14" s="88">
-        <v>0.25</v>
-      </c>
-      <c r="L14" s="76">
-        <v>60</v>
-      </c>
-      <c r="M14" s="88">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F15" s="76">
-        <v>120</v>
-      </c>
-      <c r="G15" s="88">
-        <v>0.03</v>
-      </c>
-      <c r="I15" s="76">
-        <v>180</v>
-      </c>
-      <c r="J15" s="88">
-        <v>0.1</v>
-      </c>
-      <c r="L15" s="76">
-        <v>120</v>
-      </c>
-      <c r="M15" s="88">
-        <v>0.23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F16" s="76">
-        <v>180</v>
-      </c>
-      <c r="G16" s="88">
-        <v>0.01</v>
-      </c>
-      <c r="I16" s="76">
-        <v>240</v>
-      </c>
-      <c r="J16" s="88">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="L16" s="76">
-        <v>180</v>
-      </c>
-      <c r="M16" s="88">
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="17" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F17" s="76"/>
-      <c r="G17" s="88"/>
-      <c r="I17" s="76">
-        <v>300</v>
-      </c>
-      <c r="J17" s="88">
-        <v>0.05</v>
-      </c>
-      <c r="L17" s="76">
-        <v>240</v>
-      </c>
-      <c r="M17" s="88">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="18" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F18" s="76"/>
-      <c r="G18" s="88"/>
-      <c r="I18" s="76">
-        <v>360</v>
-      </c>
-      <c r="J18" s="88">
-        <v>0.01</v>
-      </c>
-      <c r="L18" s="76">
-        <v>300</v>
-      </c>
-      <c r="M18" s="88">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="19" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F19" s="76"/>
-      <c r="G19" s="88"/>
-      <c r="I19" s="76"/>
-      <c r="J19" s="88"/>
-      <c r="L19" s="76">
-        <v>360</v>
-      </c>
-      <c r="M19" s="88">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="20" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F20" s="76"/>
-      <c r="G20" s="88"/>
-      <c r="I20" s="76"/>
-      <c r="J20" s="88"/>
-      <c r="L20" s="76">
-        <v>420</v>
-      </c>
-      <c r="M20" s="88">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="21" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F21" s="76"/>
-      <c r="G21" s="88"/>
-      <c r="I21" s="76"/>
-      <c r="J21" s="88"/>
-      <c r="L21" s="76">
-        <v>480</v>
-      </c>
-      <c r="M21" s="88">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="22" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F22" s="76"/>
-      <c r="G22" s="88"/>
-      <c r="I22" s="76"/>
-      <c r="J22" s="88"/>
-      <c r="L22" s="76"/>
-      <c r="M22" s="88"/>
-    </row>
-    <row r="23" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F23" s="76"/>
-      <c r="G23" s="88"/>
-      <c r="I23" s="76"/>
-      <c r="J23" s="88"/>
-      <c r="L23" s="76"/>
-      <c r="M23" s="88"/>
-    </row>
-    <row r="24" spans="6:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F17" s="105"/>
+      <c r="G17" s="106"/>
+    </row>
+    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F18" s="105"/>
+      <c r="G18" s="106"/>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F19" s="105"/>
+      <c r="G19" s="106"/>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F20" s="105"/>
+      <c r="G20" s="106"/>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="105"/>
+      <c r="G21" s="106"/>
+    </row>
+    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F22" s="105"/>
+      <c r="G22" s="106"/>
+    </row>
+    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F23" s="105"/>
+      <c r="G23" s="106"/>
+    </row>
+    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F24" s="86" t="s">
         <v>152</v>
       </c>
       <c r="G24" s="90">
         <f>SUM(G3:G23)</f>
         <v>1.0000000000000002</v>
-      </c>
-      <c r="I24" s="86" t="s">
-        <v>152</v>
-      </c>
-      <c r="J24" s="90">
-        <f>SUM(J3:J23)</f>
-        <v>1</v>
-      </c>
-      <c r="L24" s="86" t="s">
-        <v>152</v>
-      </c>
-      <c r="M24" s="90">
-        <f>SUM(M3:M23)</f>
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2889,8 +2621,8 @@
   </sheetPr>
   <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3002,7 +2734,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="82">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -3100,9 +2832,7 @@
   </sheetPr>
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3486,9 +3216,7 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3913,7 +3641,9 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4326,21 +4056,21 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="86" t="s">
-        <v>36</v>
+        <v>152</v>
       </c>
       <c r="B24" s="90">
         <f>SUM(B3:B23)</f>
         <v>1</v>
       </c>
       <c r="D24" s="86" t="s">
-        <v>36</v>
+        <v>152</v>
       </c>
       <c r="E24" s="90">
         <f>SUM(E3:E23)</f>
         <v>1</v>
       </c>
       <c r="G24" s="86" t="s">
-        <v>36</v>
+        <v>152</v>
       </c>
       <c r="H24" s="90">
         <f>SUM(H3:H23)</f>
@@ -8836,10 +8566,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -8859,7 +8589,7 @@
     <col min="13" max="16384" width="8.88671875" style="48"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
         <v>26</v>
       </c>
@@ -8888,7 +8618,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
         <v>27</v>
       </c>
@@ -8917,7 +8647,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="76">
         <v>0</v>
       </c>
@@ -8948,11 +8678,8 @@
       <c r="L3" s="88">
         <v>0.05</v>
       </c>
-      <c r="M3" s="48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="76">
         <v>1</v>
       </c>
@@ -8983,11 +8710,8 @@
       <c r="L4" s="88">
         <v>0.2</v>
       </c>
-      <c r="M4" s="48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="76">
         <v>2</v>
       </c>
@@ -9018,11 +8742,8 @@
       <c r="L5" s="88">
         <v>0.22</v>
       </c>
-      <c r="M5" s="48">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="76">
         <v>3</v>
       </c>
@@ -9048,11 +8769,8 @@
       <c r="L6" s="88">
         <v>0.14000000000000001</v>
       </c>
-      <c r="M6" s="48">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="76">
         <v>4</v>
       </c>
@@ -9071,11 +8789,8 @@
       <c r="L7" s="88">
         <v>0.12</v>
       </c>
-      <c r="M7" s="48">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="76">
         <v>5</v>
       </c>
@@ -9094,11 +8809,8 @@
       <c r="L8" s="88">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M8" s="48">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="76">
         <v>6</v>
       </c>
@@ -9117,11 +8829,8 @@
       <c r="L9" s="88">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M9" s="48">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="76">
         <v>7</v>
       </c>
@@ -9140,11 +8849,8 @@
       <c r="L10" s="88">
         <v>0.04</v>
       </c>
-      <c r="M10" s="48">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="76">
         <v>8</v>
       </c>
@@ -9163,11 +8869,8 @@
       <c r="L11" s="88">
         <v>0.02</v>
       </c>
-      <c r="M11" s="48">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="76">
         <v>9</v>
       </c>
@@ -9186,11 +8889,8 @@
       <c r="L12" s="88">
         <v>0.03</v>
       </c>
-      <c r="M12" s="48">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="76">
         <v>10</v>
       </c>
@@ -9209,11 +8909,8 @@
       <c r="L13" s="88">
         <v>0.02</v>
       </c>
-      <c r="M13" s="48">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="76">
         <v>11</v>
       </c>
@@ -9232,11 +8929,8 @@
       <c r="L14" s="88">
         <v>0.02</v>
       </c>
-      <c r="M14" s="48">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="76">
         <v>12</v>
       </c>
@@ -9252,7 +8946,7 @@
       <c r="K15" s="76"/>
       <c r="L15" s="88"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="76">
         <v>13</v>
       </c>
@@ -9389,21 +9083,21 @@
         <v>100</v>
       </c>
       <c r="E24" s="86" t="s">
-        <v>36</v>
+        <v>152</v>
       </c>
       <c r="F24" s="90">
         <f>SUM(F3:F23)</f>
         <v>1</v>
       </c>
       <c r="H24" s="86" t="s">
-        <v>36</v>
+        <v>152</v>
       </c>
       <c r="I24" s="90">
         <f>SUM(I3:I23)</f>
         <v>1</v>
       </c>
       <c r="K24" s="86" t="s">
-        <v>36</v>
+        <v>152</v>
       </c>
       <c r="L24" s="90">
         <f>SUM(L3:L23)</f>

</xml_diff>